<commit_message>
finished project and added report
</commit_message>
<xml_diff>
--- a/Report/Project1_data.xlsx
+++ b/Report/Project1_data.xlsx
@@ -7,7 +7,7 @@
     <workbookView windowWidth="19890" windowHeight="8355"/>
   </bookViews>
   <sheets>
-    <sheet name="parameters" sheetId="2" r:id="rId1"/>
+    <sheet name="selected values" sheetId="2" r:id="rId1"/>
     <sheet name="tau calc" sheetId="1" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
@@ -16,12 +16,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11">
   <si>
-    <t>K (bar/V)</t>
+    <t>Kp (V/bar)</t>
   </si>
   <si>
-    <t>Td (s)</t>
+    <t>Kd (V s/bar)</t>
+  </si>
+  <si>
+    <t>Ki (V/(bar s))</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>PD</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>PI</t>
+  </si>
+  <si>
+    <t>PID</t>
   </si>
   <si>
     <t>tau</t>
@@ -38,10 +56,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -53,6 +71,28 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -60,21 +100,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -90,56 +116,48 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -160,14 +178,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -183,14 +194,21 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -205,187 +223,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -399,17 +417,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -419,6 +433,21 @@
       <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -441,23 +470,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -465,8 +479,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -486,20 +500,24 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF7F7F7F"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -517,130 +535,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="25" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="27" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -992,20 +1010,71 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="B1:C1"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="5" outlineLevelCol="4"/>
+  <cols>
+    <col min="3" max="3" width="10.8571428571429" customWidth="1"/>
+    <col min="4" max="5" width="12.2857142857143" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="2:3">
-      <c r="B1" t="s">
+    <row r="1" spans="3:5">
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>9.3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -1030,22 +1099,22 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C1" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="E1" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="F1" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="H1" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -1065,7 +1134,7 @@
         <v>2.40516739176414</v>
       </c>
       <c r="H3">
-        <f>(C3+D3+E3+F3)/4</f>
+        <f t="shared" ref="H3:H10" si="0">(C3+D3+E3+F3)/4</f>
         <v>3.68629378219763</v>
       </c>
     </row>
@@ -1086,7 +1155,7 @@
         <v>2.16161841107485</v>
       </c>
       <c r="H4">
-        <f>(C4+D4+E4+F4)/4</f>
+        <f t="shared" si="0"/>
         <v>3.36945575275804</v>
       </c>
     </row>
@@ -1107,7 +1176,7 @@
         <v>2.09141896754797</v>
       </c>
       <c r="H5">
-        <f>(C5+D5+E5+F5)/4</f>
+        <f t="shared" si="0"/>
         <v>3.16975644885248</v>
       </c>
     </row>
@@ -1128,7 +1197,7 @@
         <v>2.22158241307468</v>
       </c>
       <c r="H6">
-        <f>(C6+D6+E6+F6)/4</f>
+        <f t="shared" si="0"/>
         <v>3.09292923778872</v>
       </c>
     </row>
@@ -1149,7 +1218,7 @@
         <v>2.48025586469919</v>
       </c>
       <c r="H7">
-        <f>(C7+D7+E7+F7)/4</f>
+        <f t="shared" si="0"/>
         <v>3.11581360653348</v>
       </c>
     </row>
@@ -1170,7 +1239,7 @@
         <v>2.82829789146779</v>
       </c>
       <c r="H8">
-        <f>(C8+D8+E8+F8)/4</f>
+        <f t="shared" si="0"/>
         <v>3.2262283648323</v>
       </c>
     </row>
@@ -1191,7 +1260,7 @@
         <v>3.2395829626305</v>
       </c>
       <c r="H9">
-        <f>(C9+D9+E9+F9)/4</f>
+        <f t="shared" si="0"/>
         <v>3.42714487029075</v>
       </c>
     </row>
@@ -1212,7 +1281,7 @@
         <v>3.7029160453381</v>
       </c>
       <c r="H10">
-        <f>(C10+D10+E10+F10)/4</f>
+        <f t="shared" si="0"/>
         <v>3.70930909236094</v>
       </c>
     </row>

</xml_diff>